<commit_message>
Refactor linprog.py to print optimal solution for each year
</commit_message>
<xml_diff>
--- a/附件2.xlsx
+++ b/附件2.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2024-5-1\数学建模竞赛组委会、专家组工作\竞赛2024\C题乡村农作物种植策略优化\2024-8-28-1 C题(蔡志杰)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xaz33\Desktop\Coding\git\CUMCM-2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{282A1AB1-A2F2-4147-8B0A-137D97D1BE43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7010"/>
+    <workbookView xWindow="-1695" yWindow="75" windowWidth="21825" windowHeight="13583" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2023年的农作物种植情况" sheetId="4" r:id="rId1"/>
@@ -17,8 +18,22 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2023年的农作物种植情况'!$A$1:$F$88</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2023年统计的相关数据'!$A$1:$H$108</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -2000,20 +2015,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>注：</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">(1) </t>
     </r>
     <r>
@@ -2048,21 +2049,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">(2) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>智慧大棚第一季可种植的蔬菜作物及其亩产量、种植成本和销售价格均与普通大棚相同，表中省略。</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <rPr>
         <b/>
         <sz val="12"/>
@@ -2190,6 +2176,26 @@
         <family val="1"/>
       </rPr>
       <t>)</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>注：</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(2) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>智慧大棚第一季可种植的蔬菜作物及其亩产量、种植成本和销售价格均与普通大棚相同，表中省略。</t>
     </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -2197,7 +2203,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2506,9 +2512,6 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -2518,18 +2521,21 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 10" xfId="1"/>
-    <cellStyle name="常规 27" xfId="2"/>
-    <cellStyle name="常规 34" xfId="3"/>
+    <cellStyle name="常规 10" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="常规 27" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="常规 34" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2830,23 +2836,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:F88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D117" sqref="D117"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="13.54296875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="13.54296875" style="16" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" style="7" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" style="1" customWidth="1"/>
+    <col min="1" max="3" width="13.53125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="13.53125" style="16" customWidth="1"/>
+    <col min="5" max="5" width="13.53125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="13.53125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>124</v>
       </c>
@@ -2856,7 +2864,7 @@
       <c r="C1" s="18" t="s">
         <v>196</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="26" t="s">
         <v>197</v>
       </c>
       <c r="E1" s="18" t="s">
@@ -2866,7 +2874,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>125</v>
       </c>
@@ -2886,7 +2894,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>17</v>
       </c>
@@ -2906,7 +2914,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
@@ -2926,7 +2934,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>19</v>
       </c>
@@ -2946,7 +2954,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
@@ -2966,7 +2974,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>21</v>
       </c>
@@ -2986,7 +2994,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
@@ -3006,7 +3014,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>22</v>
       </c>
@@ -3026,7 +3034,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
@@ -3046,7 +3054,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>24</v>
       </c>
@@ -3066,7 +3074,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>25</v>
       </c>
@@ -3086,7 +3094,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>26</v>
       </c>
@@ -3106,7 +3114,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>27</v>
       </c>
@@ -3126,7 +3134,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>28</v>
       </c>
@@ -3146,7 +3154,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>29</v>
       </c>
@@ -3166,7 +3174,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>30</v>
       </c>
@@ -3186,7 +3194,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>31</v>
       </c>
@@ -3206,7 +3214,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>32</v>
       </c>
@@ -3226,7 +3234,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>33</v>
       </c>
@@ -3246,7 +3254,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>34</v>
       </c>
@@ -3266,7 +3274,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>40</v>
       </c>
@@ -3286,7 +3294,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>41</v>
       </c>
@@ -3306,7 +3314,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>43</v>
       </c>
@@ -3326,7 +3334,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>44</v>
       </c>
@@ -3346,7 +3354,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>45</v>
       </c>
@@ -3366,7 +3374,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>46</v>
       </c>
@@ -3386,8 +3394,8 @@
         <v>200</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="28" t="s">
+    <row r="28" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="27" t="s">
         <v>35</v>
       </c>
       <c r="B28" s="4">
@@ -3406,8 +3414,8 @@
         <v>203</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="30"/>
+    <row r="29" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="28"/>
       <c r="B29" s="4">
         <v>36</v>
       </c>
@@ -3424,8 +3432,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="28" t="s">
+    <row r="30" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="27" t="s">
         <v>36</v>
       </c>
       <c r="B30" s="4">
@@ -3444,8 +3452,8 @@
         <v>203</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
+    <row r="31" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="28"/>
       <c r="B31" s="4">
         <v>35</v>
       </c>
@@ -3462,8 +3470,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A32" s="28" t="s">
+    <row r="32" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="27" t="s">
         <v>37</v>
       </c>
       <c r="B32" s="4">
@@ -3482,8 +3490,8 @@
         <v>203</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="30"/>
+    <row r="33" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="28"/>
       <c r="B33" s="4">
         <v>35</v>
       </c>
@@ -3500,8 +3508,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="28" t="s">
+    <row r="34" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="27" t="s">
         <v>38</v>
       </c>
       <c r="B34" s="4">
@@ -3520,8 +3528,8 @@
         <v>203</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="30"/>
+    <row r="35" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="28"/>
       <c r="B35" s="4">
         <v>35</v>
       </c>
@@ -3538,8 +3546,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="28" t="s">
+    <row r="36" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="27" t="s">
         <v>126</v>
       </c>
       <c r="B36" s="4">
@@ -3558,8 +3566,8 @@
         <v>203</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A37" s="30"/>
+    <row r="37" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="28"/>
       <c r="B37" s="4">
         <v>36</v>
       </c>
@@ -3576,8 +3584,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="28" t="s">
+    <row r="38" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="27" t="s">
         <v>39</v>
       </c>
       <c r="B38" s="4">
@@ -3596,8 +3604,8 @@
         <v>203</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A39" s="30"/>
+    <row r="39" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="28"/>
       <c r="B39" s="4">
         <v>37</v>
       </c>
@@ -3614,7 +3622,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>47</v>
       </c>
@@ -3634,7 +3642,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>48</v>
       </c>
@@ -3654,8 +3662,8 @@
         <v>200</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="28" t="s">
+    <row r="42" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="27" t="s">
         <v>94</v>
       </c>
       <c r="B42" s="4">
@@ -3674,8 +3682,8 @@
         <v>203</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A43" s="30"/>
+    <row r="43" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="28"/>
       <c r="B43" s="4">
         <v>38</v>
       </c>
@@ -3692,8 +3700,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A44" s="28" t="s">
+    <row r="44" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="27" t="s">
         <v>95</v>
       </c>
       <c r="B44" s="4">
@@ -3712,8 +3720,8 @@
         <v>203</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A45" s="30"/>
+    <row r="45" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="28"/>
       <c r="B45" s="4">
         <v>38</v>
       </c>
@@ -3730,8 +3738,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="28" t="s">
+    <row r="46" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="27" t="s">
         <v>127</v>
       </c>
       <c r="B46" s="4">
@@ -3750,8 +3758,8 @@
         <v>203</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="30"/>
+    <row r="47" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="28"/>
       <c r="B47" s="4">
         <v>38</v>
       </c>
@@ -3768,8 +3776,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A48" s="28" t="s">
+    <row r="48" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="27" t="s">
         <v>128</v>
       </c>
       <c r="B48" s="4">
@@ -3788,8 +3796,8 @@
         <v>203</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A49" s="30"/>
+    <row r="49" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="28"/>
       <c r="B49" s="4">
         <v>39</v>
       </c>
@@ -3806,8 +3814,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A50" s="28" t="s">
+    <row r="50" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="27" t="s">
         <v>96</v>
       </c>
       <c r="B50" s="4">
@@ -3826,8 +3834,8 @@
         <v>203</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="30"/>
+    <row r="51" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="28"/>
       <c r="B51" s="4">
         <v>39</v>
       </c>
@@ -3844,8 +3852,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A52" s="28" t="s">
+    <row r="52" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="27" t="s">
         <v>97</v>
       </c>
       <c r="B52" s="4">
@@ -3864,8 +3872,8 @@
         <v>203</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="30"/>
+    <row r="53" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="28"/>
       <c r="B53" s="4">
         <v>39</v>
       </c>
@@ -3882,8 +3890,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="28" t="s">
+    <row r="54" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="27" t="s">
         <v>98</v>
       </c>
       <c r="B54" s="4">
@@ -3902,8 +3910,8 @@
         <v>203</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A55" s="30"/>
+    <row r="55" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="28"/>
       <c r="B55" s="4">
         <v>40</v>
       </c>
@@ -3920,8 +3928,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A56" s="28" t="s">
+    <row r="56" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="27" t="s">
         <v>129</v>
       </c>
       <c r="B56" s="4">
@@ -3940,8 +3948,8 @@
         <v>203</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A57" s="30"/>
+    <row r="57" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="28"/>
       <c r="B57" s="4">
         <v>40</v>
       </c>
@@ -3958,8 +3966,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A58" s="28" t="s">
+    <row r="58" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="27" t="s">
         <v>99</v>
       </c>
       <c r="B58" s="4">
@@ -3978,8 +3986,8 @@
         <v>203</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A59" s="30"/>
+    <row r="59" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="28"/>
       <c r="B59" s="4">
         <v>40</v>
       </c>
@@ -3996,8 +4004,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A60" s="28" t="s">
+    <row r="60" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="27" t="s">
         <v>100</v>
       </c>
       <c r="B60" s="4">
@@ -4016,8 +4024,8 @@
         <v>203</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A61" s="30"/>
+    <row r="61" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="28"/>
       <c r="B61" s="4">
         <v>41</v>
       </c>
@@ -4034,8 +4042,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A62" s="28" t="s">
+    <row r="62" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="27" t="s">
         <v>101</v>
       </c>
       <c r="B62" s="4">
@@ -4054,8 +4062,8 @@
         <v>203</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A63" s="30"/>
+    <row r="63" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="28"/>
       <c r="B63" s="4">
         <v>41</v>
       </c>
@@ -4072,8 +4080,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A64" s="28" t="s">
+    <row r="64" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="27" t="s">
         <v>102</v>
       </c>
       <c r="B64" s="4">
@@ -4092,8 +4100,8 @@
         <v>203</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A65" s="30"/>
+    <row r="65" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="28"/>
       <c r="B65" s="4">
         <v>41</v>
       </c>
@@ -4110,8 +4118,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A66" s="28" t="s">
+    <row r="66" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="27" t="s">
         <v>103</v>
       </c>
       <c r="B66" s="4">
@@ -4130,8 +4138,8 @@
         <v>203</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A67" s="30"/>
+    <row r="67" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="28"/>
       <c r="B67" s="4">
         <v>41</v>
       </c>
@@ -4148,8 +4156,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A68" s="28" t="s">
+    <row r="68" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="27" t="s">
         <v>104</v>
       </c>
       <c r="B68" s="4">
@@ -4168,8 +4176,8 @@
         <v>203</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A69" s="30"/>
+    <row r="69" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="28"/>
       <c r="B69" s="4">
         <v>41</v>
       </c>
@@ -4186,8 +4194,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A70" s="28" t="s">
+    <row r="70" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="27" t="s">
         <v>130</v>
       </c>
       <c r="B70" s="4">
@@ -4206,7 +4214,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="29"/>
       <c r="B71" s="4">
         <v>27</v>
@@ -4224,8 +4232,8 @@
         <v>203</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A72" s="30"/>
+    <row r="72" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="28"/>
       <c r="B72" s="4">
         <v>41</v>
       </c>
@@ -4242,8 +4250,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A73" s="28" t="s">
+    <row r="73" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="27" t="s">
         <v>131</v>
       </c>
       <c r="B73" s="4">
@@ -4262,8 +4270,8 @@
         <v>203</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A74" s="30"/>
+    <row r="74" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="28"/>
       <c r="B74" s="4">
         <v>41</v>
       </c>
@@ -4280,8 +4288,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A75" s="28" t="s">
+    <row r="75" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="27" t="s">
         <v>105</v>
       </c>
       <c r="B75" s="4">
@@ -4300,7 +4308,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" s="29"/>
       <c r="B76" s="4">
         <v>33</v>
@@ -4318,7 +4326,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" s="29"/>
       <c r="B77" s="4">
         <v>24</v>
@@ -4336,8 +4344,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A78" s="30"/>
+    <row r="78" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="28"/>
       <c r="B78" s="4">
         <v>21</v>
       </c>
@@ -4354,8 +4362,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A79" s="28" t="s">
+    <row r="79" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="27" t="s">
         <v>106</v>
       </c>
       <c r="B79" s="4">
@@ -4374,7 +4382,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="29"/>
       <c r="B80" s="4">
         <v>26</v>
@@ -4392,7 +4400,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="29"/>
       <c r="B81" s="4">
         <v>22</v>
@@ -4410,8 +4418,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A82" s="30"/>
+    <row r="82" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="28"/>
       <c r="B82" s="4">
         <v>29</v>
       </c>
@@ -4428,8 +4436,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A83" s="28" t="s">
+    <row r="83" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="27" t="s">
         <v>132</v>
       </c>
       <c r="B83" s="4">
@@ -4448,7 +4456,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" s="29"/>
       <c r="B84" s="4">
         <v>28</v>
@@ -4466,8 +4474,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A85" s="30"/>
+    <row r="85" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="28"/>
       <c r="B85" s="4">
         <v>30</v>
       </c>
@@ -4484,8 +4492,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A86" s="28" t="s">
+    <row r="86" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="27" t="s">
         <v>133</v>
       </c>
       <c r="B86" s="4">
@@ -4504,7 +4512,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" s="29"/>
       <c r="B87" s="4">
         <v>34</v>
@@ -4522,8 +4530,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A88" s="30"/>
+    <row r="88" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="28"/>
       <c r="B88" s="4">
         <v>23</v>
       </c>
@@ -4541,13 +4549,19 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F88" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="红薯"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="26">
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="A86:A88"/>
+    <mergeCell ref="A75:A78"/>
+    <mergeCell ref="A79:A82"/>
+    <mergeCell ref="A70:A72"/>
     <mergeCell ref="A42:A43"/>
     <mergeCell ref="A62:A63"/>
     <mergeCell ref="A64:A65"/>
@@ -4563,11 +4577,12 @@
     <mergeCell ref="A46:A47"/>
     <mergeCell ref="A48:A49"/>
     <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A86:A88"/>
-    <mergeCell ref="A75:A78"/>
-    <mergeCell ref="A79:A82"/>
-    <mergeCell ref="A70:A72"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="A34:A35"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4576,28 +4591,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
   <dimension ref="A1:J111"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F93" sqref="F93"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.36328125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10.36328125" customWidth="1"/>
-    <col min="3" max="3" width="10.36328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.36328125" style="15" customWidth="1"/>
-    <col min="5" max="5" width="10.36328125" customWidth="1"/>
-    <col min="6" max="6" width="11.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.7265625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.46484375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" style="15" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" customWidth="1"/>
+    <col min="6" max="6" width="11.06640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.73046875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.73046875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>213</v>
       </c>
@@ -4617,13 +4634,13 @@
         <v>135</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -4649,7 +4666,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -4675,7 +4692,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -4701,7 +4718,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -4727,7 +4744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -4753,7 +4770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -4779,7 +4796,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -4805,7 +4822,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -4831,7 +4848,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -4857,7 +4874,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -4883,7 +4900,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -4909,7 +4926,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -4935,7 +4952,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -4961,7 +4978,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -4987,7 +5004,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -5013,7 +5030,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A17" s="22">
         <v>16</v>
       </c>
@@ -5039,7 +5056,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A18" s="22">
         <v>17</v>
       </c>
@@ -5065,7 +5082,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A19" s="22">
         <v>18</v>
       </c>
@@ -5091,7 +5108,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A20" s="22">
         <v>19</v>
       </c>
@@ -5117,7 +5134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A21" s="22">
         <v>20</v>
       </c>
@@ -5143,7 +5160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A22" s="22">
         <v>21</v>
       </c>
@@ -5169,7 +5186,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A23" s="22">
         <v>22</v>
       </c>
@@ -5195,7 +5212,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A24" s="22">
         <v>23</v>
       </c>
@@ -5221,7 +5238,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A25" s="22">
         <v>24</v>
       </c>
@@ -5247,7 +5264,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A26" s="22">
         <v>25</v>
       </c>
@@ -5273,7 +5290,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A27" s="22">
         <v>26</v>
       </c>
@@ -5299,7 +5316,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A28" s="22">
         <v>27</v>
       </c>
@@ -5325,7 +5342,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A29" s="22">
         <v>28</v>
       </c>
@@ -5351,7 +5368,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A30" s="22">
         <v>29</v>
       </c>
@@ -5377,7 +5394,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A31" s="22">
         <v>30</v>
       </c>
@@ -5403,7 +5420,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -5429,7 +5446,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -5455,7 +5472,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -5481,7 +5498,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>34</v>
       </c>
@@ -5507,7 +5524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>35</v>
       </c>
@@ -5533,7 +5550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>36</v>
       </c>
@@ -5559,7 +5576,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>37</v>
       </c>
@@ -5585,7 +5602,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>38</v>
       </c>
@@ -5611,7 +5628,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>39</v>
       </c>
@@ -5637,7 +5654,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>40</v>
       </c>
@@ -5663,7 +5680,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
         <v>41</v>
       </c>
@@ -5689,7 +5706,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>42</v>
       </c>
@@ -5715,7 +5732,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <v>43</v>
       </c>
@@ -5741,7 +5758,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>44</v>
       </c>
@@ -5767,7 +5784,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <v>45</v>
       </c>
@@ -5793,7 +5810,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A47" s="23">
         <v>46</v>
       </c>
@@ -5819,7 +5836,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A48" s="22">
         <v>47</v>
       </c>
@@ -5845,7 +5862,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A49" s="22">
         <v>48</v>
       </c>
@@ -5871,7 +5888,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A50" s="22">
         <v>49</v>
       </c>
@@ -5897,7 +5914,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A51" s="22">
         <v>50</v>
       </c>
@@ -5923,7 +5940,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A52" s="22">
         <v>51</v>
       </c>
@@ -5949,7 +5966,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A53" s="22">
         <v>52</v>
       </c>
@@ -5975,7 +5992,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A54" s="22">
         <v>53</v>
       </c>
@@ -6001,7 +6018,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A55" s="22">
         <v>54</v>
       </c>
@@ -6027,7 +6044,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A56" s="22">
         <v>55</v>
       </c>
@@ -6053,7 +6070,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A57" s="22">
         <v>56</v>
       </c>
@@ -6079,7 +6096,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A58" s="22">
         <v>57</v>
       </c>
@@ -6105,7 +6122,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A59" s="22">
         <v>58</v>
       </c>
@@ -6131,7 +6148,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A60" s="22">
         <v>59</v>
       </c>
@@ -6157,7 +6174,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A61" s="22">
         <v>60</v>
       </c>
@@ -6184,7 +6201,7 @@
       </c>
       <c r="J61" s="15"/>
     </row>
-    <row r="62" spans="1:10" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A62" s="22">
         <v>61</v>
       </c>
@@ -6210,7 +6227,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A63" s="22">
         <v>62</v>
       </c>
@@ -6236,7 +6253,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A64" s="22">
         <v>63</v>
       </c>
@@ -6262,7 +6279,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A65" s="22">
         <v>64</v>
       </c>
@@ -6288,7 +6305,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A66" s="4">
         <v>65</v>
       </c>
@@ -6314,7 +6331,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A67" s="4">
         <v>66</v>
       </c>
@@ -6340,7 +6357,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A68" s="4">
         <v>67</v>
       </c>
@@ -6366,7 +6383,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A69" s="4">
         <v>68</v>
       </c>
@@ -6392,7 +6409,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A70" s="4">
         <v>69</v>
       </c>
@@ -6418,7 +6435,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A71" s="4">
         <v>70</v>
       </c>
@@ -6444,7 +6461,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A72" s="4">
         <v>71</v>
       </c>
@@ -6470,7 +6487,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A73" s="4">
         <v>72</v>
       </c>
@@ -6496,7 +6513,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A74" s="4">
         <v>73</v>
       </c>
@@ -6522,7 +6539,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A75" s="4">
         <v>74</v>
       </c>
@@ -6548,7 +6565,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A76" s="4">
         <v>75</v>
       </c>
@@ -6574,7 +6591,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A77" s="4">
         <v>76</v>
       </c>
@@ -6600,7 +6617,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A78" s="4">
         <v>77</v>
       </c>
@@ -6626,7 +6643,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A79" s="4">
         <v>78</v>
       </c>
@@ -6652,7 +6669,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A80" s="4">
         <v>79</v>
       </c>
@@ -6678,7 +6695,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A81" s="4">
         <v>80</v>
       </c>
@@ -6704,7 +6721,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A82" s="4">
         <v>81</v>
       </c>
@@ -6730,7 +6747,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A83" s="4">
         <v>82</v>
       </c>
@@ -6756,7 +6773,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A84" s="22">
         <v>83</v>
       </c>
@@ -6782,7 +6799,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A85" s="22">
         <v>84</v>
       </c>
@@ -6808,7 +6825,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A86" s="22">
         <v>85</v>
       </c>
@@ -6834,7 +6851,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A87" s="4">
         <v>86</v>
       </c>
@@ -6860,7 +6877,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A88" s="4">
         <v>87</v>
       </c>
@@ -6886,7 +6903,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A89" s="4">
         <v>88</v>
       </c>
@@ -6912,7 +6929,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A90" s="4">
         <v>89</v>
       </c>
@@ -6938,7 +6955,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A91" s="22">
         <v>90</v>
       </c>
@@ -6964,7 +6981,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A92" s="22">
         <v>91</v>
       </c>
@@ -6990,7 +7007,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A93" s="22">
         <v>92</v>
       </c>
@@ -7016,7 +7033,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A94" s="22">
         <v>93</v>
       </c>
@@ -7042,7 +7059,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A95" s="22">
         <v>94</v>
       </c>
@@ -7068,7 +7085,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A96" s="22">
         <v>95</v>
       </c>
@@ -7094,7 +7111,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A97" s="22">
         <v>96</v>
       </c>
@@ -7120,7 +7137,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A98" s="22">
         <v>97</v>
       </c>
@@ -7146,7 +7163,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A99" s="22">
         <v>98</v>
       </c>
@@ -7172,7 +7189,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A100" s="22">
         <v>99</v>
       </c>
@@ -7198,7 +7215,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A101" s="22">
         <v>100</v>
       </c>
@@ -7224,7 +7241,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A102" s="22">
         <v>101</v>
       </c>
@@ -7250,7 +7267,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A103" s="22">
         <v>102</v>
       </c>
@@ -7276,7 +7293,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A104" s="22">
         <v>103</v>
       </c>
@@ -7302,7 +7319,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A105" s="22">
         <v>104</v>
       </c>
@@ -7328,7 +7345,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A106" s="22">
         <v>105</v>
       </c>
@@ -7354,7 +7371,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A107" s="22">
         <v>106</v>
       </c>
@@ -7380,7 +7397,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A108" s="22">
         <v>107</v>
       </c>
@@ -7406,22 +7423,23 @@
         <v>193</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A110" s="25" t="s">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A110" s="30" t="s">
+        <v>230</v>
+      </c>
+      <c r="B110" s="15" t="s">
         <v>227</v>
       </c>
-      <c r="B110" s="15" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A111" s="26"/>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A111" s="25"/>
       <c r="B111" s="15" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A3:H109">
+  <autoFilter ref="A1:H108" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:H109">
     <sortCondition ref="A3:A109"/>
   </sortState>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>